<commit_message>
add code for analysis
</commit_message>
<xml_diff>
--- a/multimer_results/align_res.xlsx
+++ b/multimer_results/align_res.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\U_of_T\Summer_2nd_year\lab_intern\Pardee-Lab-computation-project-pipeline\multimer_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075C0786-328A-44A7-8524-8A9352162F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A886AE-DBF7-47F7-A42E-FFEDD183B775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35055" yWindow="2355" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
   <si>
     <t>RDHMVLLEFVTAAGIT</t>
   </si>
@@ -371,6 +371,26 @@
   </si>
   <si>
     <t>score2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>score3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>explain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>score3: database &amp; GFP11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>score1: all multimer prediction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>score2: database &amp; multimer prediction</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -414,8 +434,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -696,18 +717,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E110"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="158" workbookViewId="0">
-      <selection activeCell="E102" sqref="E102"/>
+    <sheetView tabSelected="1" zoomScale="158" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="1" max="1" width="4.125" customWidth="1"/>
+    <col min="2" max="2" width="6.875" customWidth="1"/>
+    <col min="7" max="7" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -723,8 +746,14 @@
       <c r="E1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -740,8 +769,14 @@
       <c r="E2">
         <v>0.20300000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>9.06</v>
+      </c>
+      <c r="G2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -757,8 +792,14 @@
       <c r="E3">
         <v>0.20200000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>8.9949999999999992</v>
+      </c>
+      <c r="G3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -774,8 +815,14 @@
       <c r="E4">
         <v>0.19600000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>9.0679999999999996</v>
+      </c>
+      <c r="G4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -791,8 +838,11 @@
       <c r="E5">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>9.0020000000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -808,8 +858,11 @@
       <c r="E6">
         <v>0.19800000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="1">
+        <v>8.9619999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -825,8 +878,11 @@
       <c r="E7">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>1.3919999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -842,8 +898,11 @@
       <c r="E8">
         <v>0.20499999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>1.4039999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -859,8 +918,11 @@
       <c r="E9">
         <v>0.19500000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>1.6259999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -876,8 +938,11 @@
       <c r="E10">
         <v>0.192</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <v>1.659</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -893,8 +958,11 @@
       <c r="E11">
         <v>0.19700000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <v>1.1779999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -910,8 +978,11 @@
       <c r="E12">
         <v>0.19600000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <v>8.8810000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -927,8 +998,11 @@
       <c r="E13">
         <v>0.20499999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <v>9.0939999999999994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -944,8 +1018,11 @@
       <c r="E14">
         <v>0.19600000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -961,8 +1038,11 @@
       <c r="E15">
         <v>0.20399999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -978,8 +1058,11 @@
       <c r="E16">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <v>8.93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -995,8 +1078,11 @@
       <c r="E17">
         <v>0.20200000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <v>1.212</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1012,8 +1098,11 @@
       <c r="E18">
         <v>0.214</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <v>8.8539999999999992</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1029,8 +1118,11 @@
       <c r="E19">
         <v>0.19600000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <v>8.3019999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1046,8 +1138,11 @@
       <c r="E20">
         <v>0.19700000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <v>8.2550000000000008</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1063,8 +1158,11 @@
       <c r="E21">
         <v>0.19500000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <v>1.506</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1080,8 +1178,11 @@
       <c r="E22">
         <v>0.20499999999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22">
+        <v>8.4550000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1097,8 +1198,11 @@
       <c r="E23">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <v>8.4380000000000006</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1114,8 +1218,11 @@
       <c r="E24">
         <v>0.218</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <v>7.9489999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1131,8 +1238,11 @@
       <c r="E25">
         <v>0.20899999999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <v>7.82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1148,8 +1258,11 @@
       <c r="E26">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <v>8.9169999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1165,8 +1278,11 @@
       <c r="E27">
         <v>0.20300000000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <v>8.9169999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1182,8 +1298,11 @@
       <c r="E28">
         <v>0.19800000000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <v>7.9580000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1199,8 +1318,11 @@
       <c r="E29">
         <v>0.19600000000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1216,8 +1338,11 @@
       <c r="E30">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <v>8.4269999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1233,8 +1358,11 @@
       <c r="E31">
         <v>0.191</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31">
+        <v>1.825</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1250,8 +1378,11 @@
       <c r="E32">
         <v>0.19700000000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32">
+        <v>1.9530000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1267,8 +1398,11 @@
       <c r="E33">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33">
+        <v>8.8089999999999993</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1284,8 +1418,11 @@
       <c r="E34">
         <v>0.19800000000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34">
+        <v>1.359</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1301,8 +1438,11 @@
       <c r="E35">
         <v>0.183</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35">
+        <v>1.1339999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1318,8 +1458,11 @@
       <c r="E36">
         <v>0.19600000000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36">
+        <v>8.8919999999999995</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1335,8 +1478,11 @@
       <c r="E37">
         <v>0.19700000000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37">
+        <v>1.2410000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1352,8 +1498,11 @@
       <c r="E38">
         <v>0.193</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <v>1.3859999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1369,8 +1518,11 @@
       <c r="E39">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39">
+        <v>8.34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1386,8 +1538,11 @@
       <c r="E40">
         <v>0.191</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40">
+        <v>1.3919999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1403,8 +1558,11 @@
       <c r="E41">
         <v>0.187</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41">
+        <v>8.3879999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1420,8 +1578,11 @@
       <c r="E42">
         <v>0.192</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42">
+        <v>8.2880000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1437,8 +1598,11 @@
       <c r="E43">
         <v>0.19800000000000001</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43">
+        <v>1.6890000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1454,8 +1618,11 @@
       <c r="E44">
         <v>0.188</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44">
+        <v>8.1110000000000007</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1471,8 +1638,11 @@
       <c r="E45">
         <v>0.19800000000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <v>1.512</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1488,8 +1658,11 @@
       <c r="E46">
         <v>0.19700000000000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46">
+        <v>8.3070000000000004</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1505,8 +1678,11 @@
       <c r="E47">
         <v>0.20899999999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47">
+        <v>1.7090000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1522,8 +1698,11 @@
       <c r="E48">
         <v>0.19800000000000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48">
+        <v>8.218</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1539,8 +1718,11 @@
       <c r="E49">
         <v>0.191</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <v>8.2270000000000003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1556,8 +1738,11 @@
       <c r="E50">
         <v>0.19600000000000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <v>1.964</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1573,8 +1758,11 @@
       <c r="E51">
         <v>0.19900000000000001</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51">
+        <v>8.0229999999999997</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1590,8 +1778,11 @@
       <c r="E52">
         <v>0.188</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <v>2.0249999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1607,8 +1798,11 @@
       <c r="E53">
         <v>0.192</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53">
+        <v>8.7210000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1624,8 +1818,11 @@
       <c r="E54">
         <v>0.193</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54">
+        <v>8.5990000000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1641,8 +1838,11 @@
       <c r="E55">
         <v>0.19500000000000001</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55">
+        <v>1.8120000000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1658,8 +1858,11 @@
       <c r="E56">
         <v>0.193</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56">
+        <v>1.544</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1675,8 +1878,11 @@
       <c r="E57">
         <v>0.193</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57">
+        <v>7.4820000000000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1692,8 +1898,11 @@
       <c r="E58">
         <v>0.193</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58">
+        <v>1.339</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1709,8 +1918,11 @@
       <c r="E59">
         <v>0.191</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59">
+        <v>1.538</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1726,8 +1938,11 @@
       <c r="E60">
         <v>0.19900000000000001</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60">
+        <v>2.1459999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1743,8 +1958,11 @@
       <c r="E61">
         <v>0.218</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61">
+        <v>2.6429999999999998</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1760,8 +1978,11 @@
       <c r="E62">
         <v>0.192</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62">
+        <v>1.3220000000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1777,8 +1998,11 @@
       <c r="E63">
         <v>0.189</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63">
+        <v>2.4889999999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1794,8 +2018,11 @@
       <c r="E64">
         <v>0.191</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64">
+        <v>1.4910000000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1811,8 +2038,11 @@
       <c r="E65">
         <v>0.19400000000000001</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1828,8 +2058,11 @@
       <c r="E66">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66">
+        <v>1.986</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1845,8 +2078,11 @@
       <c r="E67">
         <v>0.19500000000000001</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67">
+        <v>1.633</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1862,8 +2098,11 @@
       <c r="E68">
         <v>0.19600000000000001</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68">
+        <v>1.212</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1879,8 +2118,11 @@
       <c r="E69">
         <v>0.193</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69">
+        <v>9.0020000000000007</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1896,8 +2138,11 @@
       <c r="E70">
         <v>0.20300000000000001</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70">
+        <v>2.1859999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1913,8 +2158,11 @@
       <c r="E71">
         <v>0.20399999999999999</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71">
+        <v>1.8260000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1930,8 +2178,11 @@
       <c r="E72">
         <v>0.222</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72">
+        <v>1.516</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1947,8 +2198,11 @@
       <c r="E73">
         <v>0.19900000000000001</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73" s="1">
+        <v>8.94</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1964,8 +2218,11 @@
       <c r="E74">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74">
+        <v>1.7490000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1981,8 +2238,11 @@
       <c r="E75">
         <v>0.219</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75">
+        <v>1.2949999999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1998,8 +2258,11 @@
       <c r="E76">
         <v>0.19400000000000001</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76">
+        <v>1.423</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2015,8 +2278,11 @@
       <c r="E77">
         <v>0.21099999999999999</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77">
+        <v>8.1519999999999992</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2032,8 +2298,11 @@
       <c r="E78">
         <v>0.193</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78">
+        <v>1.2909999999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2049,8 +2318,11 @@
       <c r="E79">
         <v>0.19700000000000001</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79">
+        <v>2.2770000000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2066,8 +2338,11 @@
       <c r="E80">
         <v>0.193</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80">
+        <v>1.653</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2083,8 +2358,11 @@
       <c r="E81">
         <v>0.192</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81">
+        <v>7.8920000000000003</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2100,8 +2378,11 @@
       <c r="E82">
         <v>0.19500000000000001</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82">
+        <v>1.329</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2117,8 +2398,11 @@
       <c r="E83">
         <v>0.19800000000000001</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83">
+        <v>8.7949999999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2134,8 +2418,11 @@
       <c r="E84">
         <v>0.19700000000000001</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F84">
+        <v>8.8919999999999995</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2151,8 +2438,11 @@
       <c r="E85">
         <v>0.19700000000000001</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F85">
+        <v>8.8729999999999993</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2168,8 +2458,11 @@
       <c r="E86">
         <v>0.19600000000000001</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F86">
+        <v>9.0489999999999995</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2185,8 +2478,11 @@
       <c r="E87">
         <v>0.19700000000000001</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F87">
+        <v>1.714</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2202,8 +2498,11 @@
       <c r="E88">
         <v>0.19600000000000001</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F88">
+        <v>9.0459999999999994</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2219,8 +2518,11 @@
       <c r="E89">
         <v>0.19800000000000001</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F89">
+        <v>1.677</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2236,8 +2538,11 @@
       <c r="E90">
         <v>0.19800000000000001</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F90">
+        <v>1.629</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2253,8 +2558,11 @@
       <c r="E91">
         <v>0.19400000000000001</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F91">
+        <v>1.5780000000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2270,8 +2578,11 @@
       <c r="E92">
         <v>0.193</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F92">
+        <v>7.9219999999999997</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2287,8 +2598,11 @@
       <c r="E93">
         <v>0.193</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F93">
+        <v>1.2929999999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2304,8 +2618,11 @@
       <c r="E94">
         <v>0.187</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F94">
+        <v>1.2330000000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2321,8 +2638,11 @@
       <c r="E95">
         <v>0.19600000000000001</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F95">
+        <v>1.5149999999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2338,8 +2658,11 @@
       <c r="E96">
         <v>0.19800000000000001</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F96">
+        <v>1.5049999999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2355,8 +2678,11 @@
       <c r="E97">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97">
+        <v>7.5629999999999997</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2372,8 +2698,11 @@
       <c r="E98">
         <v>0.188</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F98">
+        <v>1.758</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2389,8 +2718,11 @@
       <c r="E99">
         <v>0.19400000000000001</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F99">
+        <v>2.5920000000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2406,8 +2738,11 @@
       <c r="E100">
         <v>0.19900000000000001</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F100">
+        <v>9.0760000000000005</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2423,8 +2758,11 @@
       <c r="E101">
         <v>0.19400000000000001</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F101">
+        <v>8.9640000000000004</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2440,8 +2778,11 @@
       <c r="E102">
         <v>0.19500000000000001</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F102">
+        <v>9.0220000000000002</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -2457,8 +2798,11 @@
       <c r="E103">
         <v>0.20399999999999999</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F103">
+        <v>8.9309999999999992</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -2474,8 +2818,11 @@
       <c r="E104">
         <v>0.20399999999999999</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F104">
+        <v>1.476</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -2491,8 +2838,11 @@
       <c r="E105">
         <v>0.19900000000000001</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F105">
+        <v>9.0920000000000005</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -2508,8 +2858,11 @@
       <c r="E106">
         <v>0.19800000000000001</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F106">
+        <v>7.6539999999999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -2525,8 +2878,11 @@
       <c r="E107">
         <v>0.19600000000000001</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F107">
+        <v>1.3180000000000001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -2542,8 +2898,11 @@
       <c r="E108">
         <v>0.20499999999999999</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F108">
+        <v>1.373</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -2559,8 +2918,11 @@
       <c r="E109">
         <v>0.214</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F109">
+        <v>8.9450000000000003</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -2575,6 +2937,9 @@
       </c>
       <c r="E110">
         <v>0.19600000000000001</v>
+      </c>
+      <c r="F110">
+        <v>9.1319999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>